<commit_message>
ændret layout og fixet Estimeret tidsforbrug
Fjernet kanter og gjort det muligt at tilføje Estimeret tidsforbrug med minutter
</commit_message>
<xml_diff>
--- a/08 Project Management/Tidsregistrering/Tidsregistrering-skabelon.xlsx
+++ b/08 Project Management/Tidsregistrering/Tidsregistrering-skabelon.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ffadfded41a68b1b/Skrivebord/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikol\OneDrive\Skrivebord\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="35" documentId="8_{468DB78F-210C-4DB9-B277-7CC0D8D841D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{AECBF0C9-7974-4F0C-85A5-617ADE2A2DA3}"/>
+  <xr:revisionPtr revIDLastSave="60" documentId="8_{468DB78F-210C-4DB9-B277-7CC0D8D841D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{ECA96E5E-4074-4B8A-A4D5-65E3A23B44A7}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{84363544-26A8-43A0-AC4F-33AAA0FF1AA4}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Tidsregistrering af (Navn)</t>
   </si>
@@ -160,6 +160,9 @@
   </si>
   <si>
     <t>Timer i alt</t>
+  </si>
+  <si>
+    <t>1 time og 30 min</t>
   </si>
 </sst>
 </file>
@@ -249,7 +252,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -273,18 +276,34 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -294,46 +313,58 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Beregning" xfId="1" builtinId="22"/>
@@ -713,476 +744,485 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A07EC185-8A27-41F3-967D-179793E73F80}">
   <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" thickTop="1" thickBottom="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="53.88671875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="31.44140625" style="8" customWidth="1"/>
-    <col min="4" max="4" width="26.77734375" style="7" customWidth="1"/>
-    <col min="5" max="5" width="31" style="7" customWidth="1"/>
-    <col min="6" max="6" width="31" style="8" customWidth="1"/>
-    <col min="7" max="8" width="37.21875" style="10" customWidth="1"/>
+    <col min="1" max="2" width="53.88671875" style="13" customWidth="1"/>
+    <col min="3" max="3" width="31.44140625" style="20" customWidth="1"/>
+    <col min="4" max="4" width="26.77734375" style="19" customWidth="1"/>
+    <col min="5" max="5" width="31" style="19" customWidth="1"/>
+    <col min="6" max="6" width="31" style="24" customWidth="1"/>
+    <col min="7" max="7" width="37.21875" style="7" customWidth="1"/>
+    <col min="8" max="8" width="37.21875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="25.2" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-    </row>
-    <row r="2" spans="1:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="18" t="s">
+    <row r="1" spans="1:8" ht="24.6" x14ac:dyDescent="0.4">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+    </row>
+    <row r="2" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="A2" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="17" t="s">
+      <c r="G2" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="H2" s="17" t="s">
+      <c r="H2" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C3" s="11"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="9">
+    <row r="3" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="C3" s="14">
+        <v>43885</v>
+      </c>
+      <c r="D3" s="15"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" s="6">
         <f>E3-D3</f>
         <v>0</v>
       </c>
-      <c r="H3" s="9">
+      <c r="H3" s="1">
         <f>SUM(G$3:G3)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C4" s="3"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="9">
+    <row r="4" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="C4" s="17">
+        <v>43885</v>
+      </c>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="6">
         <f t="shared" ref="G4:G32" si="0">E4-D4</f>
         <v>0</v>
       </c>
-      <c r="H4" s="9">
+      <c r="H4" s="1">
         <f>SUM(G$3:G4)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C5" s="3"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H5" s="9">
+    <row r="5" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="C5" s="17">
+        <v>43881</v>
+      </c>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H5" s="1">
         <f>SUM(G$3:G5)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C6" s="3"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H6" s="9">
+    <row r="6" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="C6" s="17"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H6" s="1">
         <f>SUM(G$3:G6)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C7" s="3"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H7" s="9">
+    <row r="7" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="C7" s="17"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H7" s="1">
         <f>SUM(G$3:G7)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C8" s="3"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H8" s="9">
+    <row r="8" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="C8" s="17"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H8" s="1">
         <f>SUM(G$3:G8)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C9" s="3"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H9" s="9">
+    <row r="9" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="C9" s="17"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H9" s="1">
         <f>SUM(G$3:G9)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C10" s="3"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H10" s="9">
+    <row r="10" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="C10" s="17"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H10" s="1">
         <f>SUM(G$3:G10)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C11" s="3"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H11" s="9">
+    <row r="11" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="C11" s="17"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H11" s="1">
         <f>SUM(G$3:G11)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C12" s="3"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H12" s="9">
+    <row r="12" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="C12" s="17"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H12" s="1">
         <f>SUM(G$3:G12)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C13" s="3"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H13" s="9">
+    <row r="13" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="C13" s="17"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H13" s="1">
         <f>SUM(G$3:G13)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H14" s="9">
+    <row r="14" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="C14" s="17"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H14" s="1">
         <f>SUM(G$3:G14)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H15" s="9">
+    <row r="15" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="C15" s="17"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H15" s="1">
         <f>SUM(G$3:G15)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H16" s="9">
+    <row r="16" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="C16" s="17"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H16" s="1">
         <f>SUM(G$3:G16)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="3:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H17" s="9">
+    <row r="17" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="C17" s="17"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H17" s="1">
         <f>SUM(G$3:G17)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="3:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H18" s="9">
+    <row r="18" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="C18" s="17"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H18" s="1">
         <f>SUM(G$3:G18)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="3:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H19" s="9">
+    <row r="19" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="C19" s="17"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H19" s="1">
         <f>SUM(G$3:G19)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="3:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H20" s="9">
+    <row r="20" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="C20" s="17"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H20" s="1">
         <f>SUM(G$3:G20)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="3:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H21" s="9">
+    <row r="21" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="C21" s="17"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H21" s="1">
         <f>SUM(G$3:G21)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="3:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H22" s="9">
+    <row r="22" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="C22" s="17"/>
+      <c r="F22" s="23"/>
+      <c r="G22" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H22" s="1">
         <f>SUM(G$3:G22)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="3:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H23" s="9">
+    <row r="23" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="C23" s="17"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H23" s="1">
         <f>SUM(G$3:G23)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="3:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H24" s="9">
+    <row r="24" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="C24" s="17"/>
+      <c r="F24" s="23"/>
+      <c r="G24" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H24" s="1">
         <f>SUM(G$3:G24)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="3:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C25" s="3"/>
-      <c r="G25" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H25" s="9">
+    <row r="25" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="C25" s="17"/>
+      <c r="G25" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H25" s="1">
         <f>SUM(G$3:G25)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="3:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C26" s="3"/>
-      <c r="G26" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H26" s="9">
+    <row r="26" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="C26" s="17"/>
+      <c r="G26" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H26" s="1">
         <f>SUM(G$3:G26)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="3:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C27" s="3"/>
-      <c r="G27" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H27" s="9">
+    <row r="27" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="C27" s="17"/>
+      <c r="G27" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H27" s="1">
         <f>SUM(G$3:G27)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="3:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C28" s="3"/>
-      <c r="G28" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H28" s="9">
+    <row r="28" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="C28" s="17"/>
+      <c r="G28" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H28" s="1">
         <f>SUM(G$3:G28)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="3:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C29" s="3"/>
-      <c r="G29" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H29" s="9">
+    <row r="29" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="C29" s="17"/>
+      <c r="G29" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H29" s="1">
         <f>SUM(G$3:G29)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="3:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C30" s="3"/>
-      <c r="G30" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H30" s="9">
+    <row r="30" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="C30" s="17"/>
+      <c r="G30" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H30" s="1">
         <f>SUM(G$3:G30)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="3:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C31" s="3"/>
-      <c r="G31" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H31" s="9">
+    <row r="31" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="C31" s="17"/>
+      <c r="G31" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H31" s="1">
         <f>SUM(G$3:G31)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="3:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C32" s="3"/>
-      <c r="G32" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H32" s="9">
+    <row r="32" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="C32" s="17"/>
+      <c r="G32" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H32" s="1">
         <f>SUM(G$3:G32)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="3:3" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C33" s="3"/>
-    </row>
-    <row r="34" spans="3:3" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C34" s="3"/>
-    </row>
-    <row r="35" spans="3:3" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C35" s="3"/>
-    </row>
-    <row r="36" spans="3:3" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C36" s="3"/>
-    </row>
-    <row r="37" spans="3:3" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C37" s="3"/>
-    </row>
-    <row r="38" spans="3:3" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C38" s="3"/>
-    </row>
-    <row r="39" spans="3:3" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C39" s="3"/>
-    </row>
-    <row r="40" spans="3:3" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C40" s="3"/>
-    </row>
-    <row r="41" spans="3:3" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C41" s="3"/>
-    </row>
-    <row r="42" spans="3:3" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C42" s="3"/>
-    </row>
-    <row r="43" spans="3:3" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C43" s="3"/>
-    </row>
-    <row r="44" spans="3:3" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C44" s="3"/>
-    </row>
-    <row r="45" spans="3:3" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C45" s="3"/>
-    </row>
-    <row r="46" spans="3:3" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C46" s="3"/>
-    </row>
-    <row r="47" spans="3:3" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C47" s="3"/>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C33" s="17"/>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C34" s="17"/>
+    </row>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C35" s="17"/>
+    </row>
+    <row r="36" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C36" s="17"/>
+    </row>
+    <row r="37" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C37" s="17"/>
+    </row>
+    <row r="38" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C38" s="17"/>
+    </row>
+    <row r="39" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C39" s="17"/>
+    </row>
+    <row r="40" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C40" s="17"/>
+    </row>
+    <row r="41" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C41" s="17"/>
+    </row>
+    <row r="42" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C42" s="17"/>
+    </row>
+    <row r="43" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C43" s="17"/>
+    </row>
+    <row r="44" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C44" s="17"/>
+    </row>
+    <row r="45" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C45" s="17"/>
+    </row>
+    <row r="46" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C46" s="17"/>
+    </row>
+    <row r="47" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C47" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1192,11 +1232,11 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B1048576" xr:uid="{BFDCDBAC-12D7-4CE8-B28E-3FB0550AF167}">
       <formula1>Roller</formula1>
     </dataValidation>
-    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F24 C2:C1048576" xr:uid="{EAF4FEC8-302E-4BC5-B847-882BBAE51A3C}">
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576" xr:uid="{EAF4FEC8-302E-4BC5-B847-882BBAE51A3C}">
       <formula1>43881</formula1>
       <formula2>43908</formula2>
     </dataValidation>
-    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D1048576" xr:uid="{0F36D2BB-4F1D-4278-8991-092B577194F7}">
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576" xr:uid="{AAB748DE-A874-498A-B6D5-9F9C72DDE532}">
       <formula1>0.333333333333333</formula1>
       <formula2>0.708333333333333</formula2>
     </dataValidation>
@@ -1221,13 +1261,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">

</xml_diff>

<commit_message>
uploade den seneste udgave
</commit_message>
<xml_diff>
--- a/08 Project Management/Tidsregistrering/Tidsregistrering-skabelon.xlsx
+++ b/08 Project Management/Tidsregistrering/Tidsregistrering-skabelon.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikol\OneDrive\Skrivebord\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="60" documentId="8_{468DB78F-210C-4DB9-B277-7CC0D8D841D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{ECA96E5E-4074-4B8A-A4D5-65E3A23B44A7}"/>
+  <xr:revisionPtr revIDLastSave="64" documentId="8_{468DB78F-210C-4DB9-B277-7CC0D8D841D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5D48C089-D7EA-462F-831C-AFE55CD4FCA8}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{84363544-26A8-43A0-AC4F-33AAA0FF1AA4}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Tidsregistrering af (Navn)</t>
   </si>
@@ -160,9 +160,6 @@
   </si>
   <si>
     <t>Timer i alt</t>
-  </si>
-  <si>
-    <t>1 time og 30 min</t>
   </si>
 </sst>
 </file>
@@ -320,17 +317,11 @@
     <xf numFmtId="164" fontId="6" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="5" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="5" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="5" fillId="5" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -365,6 +356,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Beregning" xfId="1" builtinId="22"/>
@@ -745,52 +742,52 @@
   <dimension ref="A1:H47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="53.88671875" style="13" customWidth="1"/>
-    <col min="3" max="3" width="31.44140625" style="20" customWidth="1"/>
-    <col min="4" max="4" width="26.77734375" style="19" customWidth="1"/>
-    <col min="5" max="5" width="31" style="19" customWidth="1"/>
-    <col min="6" max="6" width="31" style="24" customWidth="1"/>
-    <col min="7" max="7" width="37.21875" style="7" customWidth="1"/>
+    <col min="1" max="2" width="53.88671875" style="11" customWidth="1"/>
+    <col min="3" max="3" width="31.44140625" style="18" customWidth="1"/>
+    <col min="4" max="4" width="26.77734375" style="17" customWidth="1"/>
+    <col min="5" max="5" width="31" style="17" customWidth="1"/>
+    <col min="6" max="6" width="31" style="22" customWidth="1"/>
+    <col min="7" max="7" width="37.21875" style="6" customWidth="1"/>
     <col min="8" max="8" width="37.21875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A1" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
+      <c r="A1" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
     </row>
     <row r="2" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="4" t="s">
         <v>36</v>
       </c>
       <c r="H2" s="3" t="s">
@@ -798,15 +795,11 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C3" s="14">
-        <v>43885</v>
-      </c>
-      <c r="D3" s="15"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="G3" s="6">
+      <c r="C3" s="12"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="5">
         <f>E3-D3</f>
         <v>0</v>
       </c>
@@ -816,13 +809,11 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C4" s="17">
-        <v>43885</v>
-      </c>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="6">
+      <c r="C4" s="15"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="5">
         <f t="shared" ref="G4:G32" si="0">E4-D4</f>
         <v>0</v>
       </c>
@@ -832,13 +823,11 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C5" s="17">
-        <v>43881</v>
-      </c>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="6">
+      <c r="C5" s="15"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -848,11 +837,11 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C6" s="17"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="6">
+      <c r="C6" s="15"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -862,11 +851,11 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C7" s="17"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="6">
+      <c r="C7" s="15"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -876,11 +865,11 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C8" s="17"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="6">
+      <c r="C8" s="15"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -890,11 +879,11 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C9" s="17"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="6">
+      <c r="C9" s="15"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -904,11 +893,11 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C10" s="17"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="6">
+      <c r="C10" s="15"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -918,11 +907,11 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C11" s="17"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="6">
+      <c r="C11" s="15"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -932,11 +921,11 @@
       </c>
     </row>
     <row r="12" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C12" s="17"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="6">
+      <c r="C12" s="15"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -946,11 +935,11 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C13" s="17"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="6">
+      <c r="C13" s="15"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -960,9 +949,9 @@
       </c>
     </row>
     <row r="14" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C14" s="17"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="6">
+      <c r="C14" s="15"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -972,9 +961,9 @@
       </c>
     </row>
     <row r="15" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C15" s="17"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="6">
+      <c r="C15" s="15"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -984,9 +973,9 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C16" s="17"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="6">
+      <c r="C16" s="15"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -996,9 +985,9 @@
       </c>
     </row>
     <row r="17" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C17" s="17"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="6">
+      <c r="C17" s="15"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1008,9 +997,9 @@
       </c>
     </row>
     <row r="18" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C18" s="17"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="6">
+      <c r="C18" s="15"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1020,9 +1009,9 @@
       </c>
     </row>
     <row r="19" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C19" s="17"/>
-      <c r="F19" s="23"/>
-      <c r="G19" s="6">
+      <c r="C19" s="15"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1032,9 +1021,9 @@
       </c>
     </row>
     <row r="20" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C20" s="17"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="6">
+      <c r="C20" s="15"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1044,9 +1033,9 @@
       </c>
     </row>
     <row r="21" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C21" s="17"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="6">
+      <c r="C21" s="15"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1056,9 +1045,9 @@
       </c>
     </row>
     <row r="22" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C22" s="17"/>
-      <c r="F22" s="23"/>
-      <c r="G22" s="6">
+      <c r="C22" s="15"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1068,9 +1057,9 @@
       </c>
     </row>
     <row r="23" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C23" s="17"/>
-      <c r="F23" s="23"/>
-      <c r="G23" s="6">
+      <c r="C23" s="15"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1080,9 +1069,9 @@
       </c>
     </row>
     <row r="24" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C24" s="17"/>
-      <c r="F24" s="23"/>
-      <c r="G24" s="6">
+      <c r="C24" s="15"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1092,8 +1081,8 @@
       </c>
     </row>
     <row r="25" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C25" s="17"/>
-      <c r="G25" s="6">
+      <c r="C25" s="15"/>
+      <c r="G25" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1103,8 +1092,8 @@
       </c>
     </row>
     <row r="26" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C26" s="17"/>
-      <c r="G26" s="6">
+      <c r="C26" s="15"/>
+      <c r="G26" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1114,8 +1103,8 @@
       </c>
     </row>
     <row r="27" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C27" s="17"/>
-      <c r="G27" s="6">
+      <c r="C27" s="15"/>
+      <c r="G27" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1125,8 +1114,8 @@
       </c>
     </row>
     <row r="28" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C28" s="17"/>
-      <c r="G28" s="6">
+      <c r="C28" s="15"/>
+      <c r="G28" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1136,8 +1125,8 @@
       </c>
     </row>
     <row r="29" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C29" s="17"/>
-      <c r="G29" s="6">
+      <c r="C29" s="15"/>
+      <c r="G29" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1147,8 +1136,8 @@
       </c>
     </row>
     <row r="30" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C30" s="17"/>
-      <c r="G30" s="6">
+      <c r="C30" s="15"/>
+      <c r="G30" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1158,8 +1147,8 @@
       </c>
     </row>
     <row r="31" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C31" s="17"/>
-      <c r="G31" s="6">
+      <c r="C31" s="15"/>
+      <c r="G31" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1169,8 +1158,8 @@
       </c>
     </row>
     <row r="32" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C32" s="17"/>
-      <c r="G32" s="6">
+      <c r="C32" s="15"/>
+      <c r="G32" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1180,49 +1169,49 @@
       </c>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C33" s="17"/>
+      <c r="C33" s="15"/>
     </row>
     <row r="34" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C34" s="17"/>
+      <c r="C34" s="15"/>
     </row>
     <row r="35" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C35" s="17"/>
+      <c r="C35" s="15"/>
     </row>
     <row r="36" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C36" s="17"/>
+      <c r="C36" s="15"/>
     </row>
     <row r="37" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C37" s="17"/>
+      <c r="C37" s="15"/>
     </row>
     <row r="38" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C38" s="17"/>
+      <c r="C38" s="15"/>
     </row>
     <row r="39" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C39" s="17"/>
+      <c r="C39" s="15"/>
     </row>
     <row r="40" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C40" s="17"/>
+      <c r="C40" s="15"/>
     </row>
     <row r="41" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C41" s="17"/>
+      <c r="C41" s="15"/>
     </row>
     <row r="42" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C42" s="17"/>
+      <c r="C42" s="15"/>
     </row>
     <row r="43" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C43" s="17"/>
+      <c r="C43" s="15"/>
     </row>
     <row r="44" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C44" s="17"/>
+      <c r="C44" s="15"/>
     </row>
     <row r="45" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C45" s="17"/>
+      <c r="C45" s="15"/>
     </row>
     <row r="46" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C46" s="17"/>
+      <c r="C46" s="15"/>
     </row>
     <row r="47" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C47" s="17"/>
+      <c r="C47" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1261,13 +1250,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">

</xml_diff>